<commit_message>
Last Update 27-12-2018 14:37:06.75
</commit_message>
<xml_diff>
--- a/Acadamic Log Book MC-18-19.xlsx
+++ b/Acadamic Log Book MC-18-19.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="15600" windowHeight="7950" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="15600" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="Attendance" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="123">
   <si>
     <t>S.NO</t>
   </si>
@@ -772,59 +772,32 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="17" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="1" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="1" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="1" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="1" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -838,6 +811,72 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -849,45 +888,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -895,7 +895,27 @@
     <cellStyle name="Normal 2" xfId="1"/>
     <cellStyle name="Normal 3" xfId="2"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -937,18 +957,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1254,11 +1262,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BN52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="D27" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="4" topLeftCell="D36" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4:D4"/>
+      <selection pane="bottomRight" activeCell="L8" sqref="L8:L50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1273,42 +1281,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:66" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="39"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="61"/>
       <c r="E1" s="20" t="s">
         <v>6</v>
       </c>
       <c r="F1" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="42" t="s">
+      <c r="G1" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="65" t="s">
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="65"/>
-      <c r="M1" s="65"/>
-      <c r="N1" s="65"/>
-      <c r="O1" s="50" t="s">
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="57" t="s">
         <v>121</v>
       </c>
-      <c r="P1" s="51"/>
-      <c r="Q1" s="51"/>
-      <c r="R1" s="51"/>
-      <c r="S1" s="51"/>
-      <c r="T1" s="51"/>
-      <c r="U1" s="51"/>
-      <c r="V1" s="51"/>
-      <c r="W1" s="51"/>
-      <c r="X1" s="52"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
+      <c r="R1" s="58"/>
+      <c r="S1" s="58"/>
+      <c r="T1" s="58"/>
+      <c r="U1" s="58"/>
+      <c r="V1" s="58"/>
+      <c r="W1" s="58"/>
+      <c r="X1" s="59"/>
       <c r="Y1" s="25"/>
       <c r="Z1" s="25"/>
       <c r="AA1" s="25"/>
@@ -1321,12 +1329,12 @@
       <c r="AH1" s="25"/>
     </row>
     <row r="2" spans="1:66" ht="19.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="41"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="63"/>
       <c r="E2" s="11" t="s">
         <v>8</v>
       </c>
@@ -1339,24 +1347,24 @@
       <c r="H2" s="45"/>
       <c r="I2" s="45"/>
       <c r="J2" s="45"/>
-      <c r="K2" s="65" t="s">
+      <c r="K2" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="65"/>
-      <c r="M2" s="65"/>
-      <c r="N2" s="65"/>
-      <c r="O2" s="49" t="s">
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="56" t="s">
         <v>120</v>
       </c>
-      <c r="P2" s="49"/>
-      <c r="Q2" s="49"/>
-      <c r="R2" s="49"/>
-      <c r="S2" s="49"/>
-      <c r="T2" s="49"/>
-      <c r="U2" s="49"/>
-      <c r="V2" s="49"/>
-      <c r="W2" s="49"/>
-      <c r="X2" s="49"/>
+      <c r="P2" s="56"/>
+      <c r="Q2" s="56"/>
+      <c r="R2" s="56"/>
+      <c r="S2" s="56"/>
+      <c r="T2" s="56"/>
+      <c r="U2" s="56"/>
+      <c r="V2" s="56"/>
+      <c r="W2" s="56"/>
+      <c r="X2" s="56"/>
       <c r="Y2" s="25"/>
       <c r="Z2" s="25"/>
       <c r="AA2" s="25"/>
@@ -1369,12 +1377,12 @@
       <c r="AH2" s="25"/>
     </row>
     <row r="3" spans="1:66" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="60" t="s">
         <v>122</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="39"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="61"/>
       <c r="E3" s="24" t="s">
         <v>19</v>
       </c>
@@ -1387,24 +1395,24 @@
       <c r="H3" s="45"/>
       <c r="I3" s="45"/>
       <c r="J3" s="45"/>
-      <c r="K3" s="65" t="s">
+      <c r="K3" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="65"/>
-      <c r="M3" s="65"/>
-      <c r="N3" s="65"/>
-      <c r="O3" s="49" t="s">
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="P3" s="49"/>
-      <c r="Q3" s="49"/>
-      <c r="R3" s="49"/>
-      <c r="S3" s="49"/>
-      <c r="T3" s="49"/>
-      <c r="U3" s="49"/>
-      <c r="V3" s="49"/>
-      <c r="W3" s="49"/>
-      <c r="X3" s="49"/>
+      <c r="P3" s="56"/>
+      <c r="Q3" s="56"/>
+      <c r="R3" s="56"/>
+      <c r="S3" s="56"/>
+      <c r="T3" s="56"/>
+      <c r="U3" s="56"/>
+      <c r="V3" s="56"/>
+      <c r="W3" s="56"/>
+      <c r="X3" s="56"/>
       <c r="Y3" s="26"/>
       <c r="Z3" s="26"/>
       <c r="AA3" s="26"/>
@@ -1417,56 +1425,56 @@
       <c r="AH3" s="26"/>
     </row>
     <row r="4" spans="1:66" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="46">
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="42">
         <v>43070</v>
       </c>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="47"/>
-      <c r="M4" s="47"/>
-      <c r="N4" s="47"/>
-      <c r="O4" s="47"/>
-      <c r="P4" s="47"/>
-      <c r="Q4" s="47"/>
-      <c r="R4" s="47"/>
-      <c r="S4" s="47"/>
-      <c r="T4" s="47"/>
-      <c r="U4" s="47"/>
-      <c r="V4" s="47"/>
-      <c r="W4" s="47"/>
-      <c r="X4" s="48"/>
-      <c r="Y4" s="46"/>
-      <c r="Z4" s="47"/>
-      <c r="AA4" s="47"/>
-      <c r="AB4" s="47"/>
-      <c r="AC4" s="47"/>
-      <c r="AD4" s="47"/>
-      <c r="AE4" s="47"/>
-      <c r="AF4" s="47"/>
-      <c r="AG4" s="47"/>
-      <c r="AH4" s="47"/>
-      <c r="AI4" s="47"/>
-      <c r="AJ4" s="47"/>
-      <c r="AK4" s="47"/>
-      <c r="AL4" s="47"/>
-      <c r="AM4" s="47"/>
-      <c r="AN4" s="47"/>
-      <c r="AO4" s="47"/>
-      <c r="AP4" s="47"/>
-      <c r="AQ4" s="47"/>
-      <c r="AR4" s="47"/>
-      <c r="AS4" s="47"/>
-      <c r="AT4" s="48"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="43"/>
+      <c r="K4" s="43"/>
+      <c r="L4" s="43"/>
+      <c r="M4" s="43"/>
+      <c r="N4" s="43"/>
+      <c r="O4" s="43"/>
+      <c r="P4" s="43"/>
+      <c r="Q4" s="43"/>
+      <c r="R4" s="43"/>
+      <c r="S4" s="43"/>
+      <c r="T4" s="43"/>
+      <c r="U4" s="43"/>
+      <c r="V4" s="43"/>
+      <c r="W4" s="43"/>
+      <c r="X4" s="44"/>
+      <c r="Y4" s="42"/>
+      <c r="Z4" s="43"/>
+      <c r="AA4" s="43"/>
+      <c r="AB4" s="43"/>
+      <c r="AC4" s="43"/>
+      <c r="AD4" s="43"/>
+      <c r="AE4" s="43"/>
+      <c r="AF4" s="43"/>
+      <c r="AG4" s="43"/>
+      <c r="AH4" s="43"/>
+      <c r="AI4" s="43"/>
+      <c r="AJ4" s="43"/>
+      <c r="AK4" s="43"/>
+      <c r="AL4" s="43"/>
+      <c r="AM4" s="43"/>
+      <c r="AN4" s="43"/>
+      <c r="AO4" s="43"/>
+      <c r="AP4" s="43"/>
+      <c r="AQ4" s="43"/>
+      <c r="AR4" s="43"/>
+      <c r="AS4" s="43"/>
+      <c r="AT4" s="44"/>
       <c r="AU4" s="27"/>
       <c r="AV4" s="27"/>
       <c r="AW4" s="27"/>
@@ -1489,13 +1497,13 @@
       <c r="BN4" s="27"/>
     </row>
     <row r="5" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="55" t="s">
+      <c r="C5" s="46" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="9" t="s">
@@ -1522,7 +1530,9 @@
       <c r="K5" s="35">
         <v>12</v>
       </c>
-      <c r="L5" s="35"/>
+      <c r="L5" s="35">
+        <v>12</v>
+      </c>
       <c r="M5" s="35"/>
       <c r="N5" s="35"/>
       <c r="O5" s="35"/>
@@ -1579,9 +1589,9 @@
       <c r="BN5" s="35"/>
     </row>
     <row r="6" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A6" s="37"/>
-      <c r="B6" s="37"/>
-      <c r="C6" s="56"/>
+      <c r="A6" s="49"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="47"/>
       <c r="D6" s="9" t="s">
         <v>1</v>
       </c>
@@ -1606,7 +1616,9 @@
       <c r="K6" s="35">
         <v>22</v>
       </c>
-      <c r="L6" s="35"/>
+      <c r="L6" s="35">
+        <v>26</v>
+      </c>
       <c r="M6" s="35"/>
       <c r="N6" s="35"/>
       <c r="O6" s="35"/>
@@ -1663,11 +1675,11 @@
       <c r="BN6" s="35"/>
     </row>
     <row r="7" spans="1:66" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="37"/>
+      <c r="A7" s="49"/>
       <c r="B7" s="23" t="s">
         <v>119</v>
       </c>
-      <c r="C7" s="57"/>
+      <c r="C7" s="48"/>
       <c r="D7" s="10" t="s">
         <v>2</v>
       </c>
@@ -1692,7 +1704,9 @@
       <c r="K7" s="35">
         <v>2</v>
       </c>
-      <c r="L7" s="35"/>
+      <c r="L7" s="35">
+        <v>1</v>
+      </c>
       <c r="M7" s="35"/>
       <c r="N7" s="35"/>
       <c r="O7" s="35"/>
@@ -1752,10 +1766,10 @@
       <c r="A8" s="34">
         <v>1</v>
       </c>
-      <c r="B8" s="73" t="s">
+      <c r="B8" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="73" t="s">
+      <c r="C8" s="38" t="s">
         <v>34</v>
       </c>
       <c r="D8" s="5"/>
@@ -1766,7 +1780,9 @@
       <c r="I8" s="32"/>
       <c r="J8" s="35"/>
       <c r="K8" s="36"/>
-      <c r="L8" s="36"/>
+      <c r="L8" s="36" t="s">
+        <v>6</v>
+      </c>
       <c r="M8" s="36"/>
       <c r="N8" s="35"/>
       <c r="O8" s="36"/>
@@ -1826,10 +1842,10 @@
       <c r="A9" s="34">
         <v>2</v>
       </c>
-      <c r="B9" s="73" t="s">
+      <c r="B9" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="73" t="s">
+      <c r="C9" s="38" t="s">
         <v>36</v>
       </c>
       <c r="D9" s="4"/>
@@ -1840,7 +1856,9 @@
       <c r="I9" s="32"/>
       <c r="J9" s="35"/>
       <c r="K9" s="36"/>
-      <c r="L9" s="36"/>
+      <c r="L9" s="36" t="s">
+        <v>6</v>
+      </c>
       <c r="M9" s="36"/>
       <c r="N9" s="35"/>
       <c r="O9" s="36"/>
@@ -1900,10 +1918,10 @@
       <c r="A10" s="34">
         <v>3</v>
       </c>
-      <c r="B10" s="73" t="s">
+      <c r="B10" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="73" t="s">
+      <c r="C10" s="38" t="s">
         <v>38</v>
       </c>
       <c r="D10" s="4"/>
@@ -1914,7 +1932,9 @@
       <c r="I10" s="32"/>
       <c r="J10" s="35"/>
       <c r="K10" s="35"/>
-      <c r="L10" s="35"/>
+      <c r="L10" s="36" t="s">
+        <v>6</v>
+      </c>
       <c r="M10" s="36"/>
       <c r="N10" s="36"/>
       <c r="O10" s="36"/>
@@ -1974,10 +1994,10 @@
       <c r="A11" s="34">
         <v>4</v>
       </c>
-      <c r="B11" s="73" t="s">
+      <c r="B11" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="73" t="s">
+      <c r="C11" s="38" t="s">
         <v>40</v>
       </c>
       <c r="D11" s="5"/>
@@ -1988,7 +2008,9 @@
       <c r="I11" s="32"/>
       <c r="J11" s="36"/>
       <c r="K11" s="36"/>
-      <c r="L11" s="36"/>
+      <c r="L11" s="36" t="s">
+        <v>6</v>
+      </c>
       <c r="M11" s="35"/>
       <c r="N11" s="36"/>
       <c r="O11" s="36"/>
@@ -2048,10 +2070,10 @@
       <c r="A12" s="34">
         <v>5</v>
       </c>
-      <c r="B12" s="73" t="s">
+      <c r="B12" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="73" t="s">
+      <c r="C12" s="38" t="s">
         <v>42</v>
       </c>
       <c r="D12" s="4"/>
@@ -2062,7 +2084,9 @@
       <c r="I12" s="32"/>
       <c r="J12" s="36"/>
       <c r="K12" s="36"/>
-      <c r="L12" s="36"/>
+      <c r="L12" s="36" t="s">
+        <v>6</v>
+      </c>
       <c r="M12" s="36"/>
       <c r="N12" s="36"/>
       <c r="O12" s="36"/>
@@ -2122,10 +2146,10 @@
       <c r="A13" s="34">
         <v>6</v>
       </c>
-      <c r="B13" s="73" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" s="73" t="s">
+      <c r="B13" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="38" t="s">
         <v>44</v>
       </c>
       <c r="D13" s="4"/>
@@ -2136,7 +2160,9 @@
       <c r="I13" s="32"/>
       <c r="J13" s="36"/>
       <c r="K13" s="36"/>
-      <c r="L13" s="36"/>
+      <c r="L13" s="36" t="s">
+        <v>6</v>
+      </c>
       <c r="M13" s="36"/>
       <c r="N13" s="35"/>
       <c r="O13" s="36"/>
@@ -2196,10 +2222,10 @@
       <c r="A14" s="34">
         <v>7</v>
       </c>
-      <c r="B14" s="73" t="s">
+      <c r="B14" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="73" t="s">
+      <c r="C14" s="38" t="s">
         <v>46</v>
       </c>
       <c r="D14" s="4"/>
@@ -2210,7 +2236,9 @@
       <c r="I14" s="32"/>
       <c r="J14" s="36"/>
       <c r="K14" s="36"/>
-      <c r="L14" s="36"/>
+      <c r="L14" s="36" t="s">
+        <v>6</v>
+      </c>
       <c r="M14" s="35"/>
       <c r="N14" s="36"/>
       <c r="O14" s="36"/>
@@ -2270,10 +2298,10 @@
       <c r="A15" s="34">
         <v>8</v>
       </c>
-      <c r="B15" s="73" t="s">
+      <c r="B15" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="73" t="s">
+      <c r="C15" s="38" t="s">
         <v>48</v>
       </c>
       <c r="D15" s="4"/>
@@ -2284,7 +2312,9 @@
       <c r="I15" s="32"/>
       <c r="J15" s="36"/>
       <c r="K15" s="36"/>
-      <c r="L15" s="36"/>
+      <c r="L15" s="36" t="s">
+        <v>6</v>
+      </c>
       <c r="M15" s="36"/>
       <c r="N15" s="36"/>
       <c r="O15" s="36"/>
@@ -2344,10 +2374,10 @@
       <c r="A16" s="34">
         <v>9</v>
       </c>
-      <c r="B16" s="73" t="s">
+      <c r="B16" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="73" t="s">
+      <c r="C16" s="38" t="s">
         <v>50</v>
       </c>
       <c r="D16" s="4"/>
@@ -2358,7 +2388,9 @@
       <c r="I16" s="32"/>
       <c r="J16" s="36"/>
       <c r="K16" s="36"/>
-      <c r="L16" s="36"/>
+      <c r="L16" s="36" t="s">
+        <v>6</v>
+      </c>
       <c r="M16" s="35"/>
       <c r="N16" s="35"/>
       <c r="O16" s="36"/>
@@ -2418,10 +2450,10 @@
       <c r="A17" s="34">
         <v>10</v>
       </c>
-      <c r="B17" s="73" t="s">
+      <c r="B17" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="C17" s="73" t="s">
+      <c r="C17" s="38" t="s">
         <v>52</v>
       </c>
       <c r="D17" s="4"/>
@@ -2432,7 +2464,9 @@
       <c r="I17" s="32"/>
       <c r="J17" s="36"/>
       <c r="K17" s="36"/>
-      <c r="L17" s="36"/>
+      <c r="L17" s="36" t="s">
+        <v>6</v>
+      </c>
       <c r="M17" s="36"/>
       <c r="N17" s="36"/>
       <c r="O17" s="35"/>
@@ -2492,10 +2526,10 @@
       <c r="A18" s="34">
         <v>11</v>
       </c>
-      <c r="B18" s="73" t="s">
+      <c r="B18" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="73" t="s">
+      <c r="C18" s="38" t="s">
         <v>54</v>
       </c>
       <c r="D18" s="4"/>
@@ -2506,7 +2540,9 @@
       <c r="I18" s="32"/>
       <c r="J18" s="36"/>
       <c r="K18" s="36"/>
-      <c r="L18" s="36"/>
+      <c r="L18" s="36" t="s">
+        <v>6</v>
+      </c>
       <c r="M18" s="36"/>
       <c r="N18" s="36"/>
       <c r="O18" s="35"/>
@@ -2566,10 +2602,10 @@
       <c r="A19" s="34">
         <v>12</v>
       </c>
-      <c r="B19" s="73" t="s">
+      <c r="B19" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="C19" s="73" t="s">
+      <c r="C19" s="38" t="s">
         <v>56</v>
       </c>
       <c r="D19" s="4"/>
@@ -2580,7 +2616,9 @@
       <c r="I19" s="32"/>
       <c r="J19" s="36"/>
       <c r="K19" s="36"/>
-      <c r="L19" s="36"/>
+      <c r="L19" s="36" t="s">
+        <v>6</v>
+      </c>
       <c r="M19" s="36"/>
       <c r="N19" s="36"/>
       <c r="O19" s="36"/>
@@ -2640,10 +2678,10 @@
       <c r="A20" s="34">
         <v>13</v>
       </c>
-      <c r="B20" s="73" t="s">
+      <c r="B20" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="73" t="s">
+      <c r="C20" s="38" t="s">
         <v>58</v>
       </c>
       <c r="D20" s="4"/>
@@ -2654,7 +2692,9 @@
       <c r="I20" s="32"/>
       <c r="J20" s="36"/>
       <c r="K20" s="36"/>
-      <c r="L20" s="36"/>
+      <c r="L20" s="36" t="s">
+        <v>6</v>
+      </c>
       <c r="M20" s="36"/>
       <c r="N20" s="36"/>
       <c r="O20" s="36"/>
@@ -2714,10 +2754,10 @@
       <c r="A21" s="34">
         <v>14</v>
       </c>
-      <c r="B21" s="73" t="s">
+      <c r="B21" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="73" t="s">
+      <c r="C21" s="38" t="s">
         <v>60</v>
       </c>
       <c r="D21" s="6"/>
@@ -2728,7 +2768,9 @@
       <c r="I21" s="32"/>
       <c r="J21" s="36"/>
       <c r="K21" s="36"/>
-      <c r="L21" s="36"/>
+      <c r="L21" s="36" t="s">
+        <v>6</v>
+      </c>
       <c r="M21" s="35"/>
       <c r="N21" s="35"/>
       <c r="O21" s="36"/>
@@ -2788,10 +2830,10 @@
       <c r="A22" s="34">
         <v>15</v>
       </c>
-      <c r="B22" s="73" t="s">
+      <c r="B22" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="73" t="s">
+      <c r="C22" s="38" t="s">
         <v>62</v>
       </c>
       <c r="D22" s="13"/>
@@ -2802,7 +2844,9 @@
       <c r="I22" s="32"/>
       <c r="J22" s="36"/>
       <c r="K22" s="36"/>
-      <c r="L22" s="36"/>
+      <c r="L22" s="36" t="s">
+        <v>6</v>
+      </c>
       <c r="M22" s="36"/>
       <c r="N22" s="36"/>
       <c r="O22" s="36"/>
@@ -2862,10 +2906,10 @@
       <c r="A23" s="34">
         <v>16</v>
       </c>
-      <c r="B23" s="73" t="s">
+      <c r="B23" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="C23" s="73" t="s">
+      <c r="C23" s="38" t="s">
         <v>64</v>
       </c>
       <c r="D23" s="4"/>
@@ -2876,7 +2920,9 @@
       <c r="I23" s="32"/>
       <c r="J23" s="36"/>
       <c r="K23" s="36"/>
-      <c r="L23" s="36"/>
+      <c r="L23" s="36" t="s">
+        <v>6</v>
+      </c>
       <c r="M23" s="35"/>
       <c r="N23" s="35"/>
       <c r="O23" s="36"/>
@@ -2936,10 +2982,10 @@
       <c r="A24" s="34">
         <v>17</v>
       </c>
-      <c r="B24" s="73" t="s">
+      <c r="B24" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="C24" s="73" t="s">
+      <c r="C24" s="38" t="s">
         <v>66</v>
       </c>
       <c r="D24" s="4"/>
@@ -2950,7 +2996,9 @@
       <c r="I24" s="32"/>
       <c r="J24" s="35"/>
       <c r="K24" s="36"/>
-      <c r="L24" s="36"/>
+      <c r="L24" s="36" t="s">
+        <v>6</v>
+      </c>
       <c r="M24" s="36"/>
       <c r="N24" s="35"/>
       <c r="O24" s="35"/>
@@ -3010,10 +3058,10 @@
       <c r="A25" s="34">
         <v>18</v>
       </c>
-      <c r="B25" s="73" t="s">
+      <c r="B25" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="C25" s="73" t="s">
+      <c r="C25" s="38" t="s">
         <v>68</v>
       </c>
       <c r="D25" s="4"/>
@@ -3024,7 +3072,9 @@
       <c r="I25" s="32"/>
       <c r="J25" s="36"/>
       <c r="K25" s="36"/>
-      <c r="L25" s="36"/>
+      <c r="L25" s="36" t="s">
+        <v>6</v>
+      </c>
       <c r="M25" s="36"/>
       <c r="N25" s="36"/>
       <c r="O25" s="36"/>
@@ -3084,10 +3134,10 @@
       <c r="A26" s="34">
         <v>19</v>
       </c>
-      <c r="B26" s="73" t="s">
+      <c r="B26" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="C26" s="73" t="s">
+      <c r="C26" s="38" t="s">
         <v>70</v>
       </c>
       <c r="D26" s="4"/>
@@ -3098,7 +3148,9 @@
       <c r="I26" s="32"/>
       <c r="J26" s="36"/>
       <c r="K26" s="36"/>
-      <c r="L26" s="36"/>
+      <c r="L26" s="36" t="s">
+        <v>6</v>
+      </c>
       <c r="M26" s="36"/>
       <c r="N26" s="36"/>
       <c r="O26" s="36"/>
@@ -3158,10 +3210,10 @@
       <c r="A27" s="34">
         <v>20</v>
       </c>
-      <c r="B27" s="73" t="s">
+      <c r="B27" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="C27" s="73" t="s">
+      <c r="C27" s="38" t="s">
         <v>72</v>
       </c>
       <c r="D27" s="4"/>
@@ -3172,7 +3224,9 @@
       <c r="I27" s="32"/>
       <c r="J27" s="36"/>
       <c r="K27" s="36"/>
-      <c r="L27" s="36"/>
+      <c r="L27" s="36" t="s">
+        <v>6</v>
+      </c>
       <c r="M27" s="36"/>
       <c r="N27" s="36"/>
       <c r="O27" s="36"/>
@@ -3232,10 +3286,10 @@
       <c r="A28" s="34">
         <v>21</v>
       </c>
-      <c r="B28" s="73" t="s">
+      <c r="B28" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="C28" s="73" t="s">
+      <c r="C28" s="38" t="s">
         <v>74</v>
       </c>
       <c r="D28" s="4"/>
@@ -3246,7 +3300,9 @@
       <c r="I28" s="32"/>
       <c r="J28" s="35"/>
       <c r="K28" s="36"/>
-      <c r="L28" s="36"/>
+      <c r="L28" s="36" t="s">
+        <v>6</v>
+      </c>
       <c r="M28" s="36"/>
       <c r="N28" s="36"/>
       <c r="O28" s="36"/>
@@ -3306,10 +3362,10 @@
       <c r="A29" s="34">
         <v>22</v>
       </c>
-      <c r="B29" s="73" t="s">
+      <c r="B29" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="C29" s="73" t="s">
+      <c r="C29" s="38" t="s">
         <v>76</v>
       </c>
       <c r="D29" s="4"/>
@@ -3320,7 +3376,9 @@
       <c r="I29" s="32"/>
       <c r="J29" s="36"/>
       <c r="K29" s="36"/>
-      <c r="L29" s="36"/>
+      <c r="L29" s="36" t="s">
+        <v>6</v>
+      </c>
       <c r="M29" s="36"/>
       <c r="N29" s="36"/>
       <c r="O29" s="36"/>
@@ -3380,10 +3438,10 @@
       <c r="A30" s="34">
         <v>23</v>
       </c>
-      <c r="B30" s="73" t="s">
+      <c r="B30" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="C30" s="73" t="s">
+      <c r="C30" s="38" t="s">
         <v>78</v>
       </c>
       <c r="D30" s="7"/>
@@ -3394,7 +3452,9 @@
       <c r="I30" s="32"/>
       <c r="J30" s="35"/>
       <c r="K30" s="36"/>
-      <c r="L30" s="36"/>
+      <c r="L30" s="36" t="s">
+        <v>6</v>
+      </c>
       <c r="M30" s="36"/>
       <c r="N30" s="36"/>
       <c r="O30" s="36"/>
@@ -3454,10 +3514,10 @@
       <c r="A31" s="34">
         <v>24</v>
       </c>
-      <c r="B31" s="73" t="s">
+      <c r="B31" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="C31" s="73" t="s">
+      <c r="C31" s="38" t="s">
         <v>80</v>
       </c>
       <c r="D31" s="8"/>
@@ -3468,7 +3528,9 @@
       <c r="I31" s="32"/>
       <c r="J31" s="36"/>
       <c r="K31" s="36"/>
-      <c r="L31" s="36"/>
+      <c r="L31" s="36" t="s">
+        <v>6</v>
+      </c>
       <c r="M31" s="36"/>
       <c r="N31" s="36"/>
       <c r="O31" s="36"/>
@@ -3528,10 +3590,10 @@
       <c r="A32" s="34">
         <v>25</v>
       </c>
-      <c r="B32" s="73" t="s">
+      <c r="B32" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="C32" s="73" t="s">
+      <c r="C32" s="38" t="s">
         <v>82</v>
       </c>
       <c r="D32" s="6"/>
@@ -3542,7 +3604,9 @@
       <c r="I32" s="32"/>
       <c r="J32" s="36"/>
       <c r="K32" s="36"/>
-      <c r="L32" s="36"/>
+      <c r="L32" s="36" t="s">
+        <v>6</v>
+      </c>
       <c r="M32" s="36"/>
       <c r="N32" s="35"/>
       <c r="O32" s="36"/>
@@ -3602,10 +3666,10 @@
       <c r="A33" s="34">
         <v>26</v>
       </c>
-      <c r="B33" s="73" t="s">
+      <c r="B33" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="C33" s="73" t="s">
+      <c r="C33" s="38" t="s">
         <v>84</v>
       </c>
       <c r="D33" s="4"/>
@@ -3616,7 +3680,9 @@
       <c r="I33" s="32"/>
       <c r="J33" s="36"/>
       <c r="K33" s="36"/>
-      <c r="L33" s="36"/>
+      <c r="L33" s="36" t="s">
+        <v>6</v>
+      </c>
       <c r="M33" s="36"/>
       <c r="N33" s="36"/>
       <c r="O33" s="36"/>
@@ -3676,10 +3742,10 @@
       <c r="A34" s="34">
         <v>27</v>
       </c>
-      <c r="B34" s="73" t="s">
+      <c r="B34" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="C34" s="73" t="s">
+      <c r="C34" s="38" t="s">
         <v>86</v>
       </c>
       <c r="D34" s="8"/>
@@ -3690,7 +3756,9 @@
       <c r="I34" s="32"/>
       <c r="J34" s="35"/>
       <c r="K34" s="36"/>
-      <c r="L34" s="36"/>
+      <c r="L34" s="36" t="s">
+        <v>6</v>
+      </c>
       <c r="M34" s="36"/>
       <c r="N34" s="36"/>
       <c r="O34" s="36"/>
@@ -3750,10 +3818,10 @@
       <c r="A35" s="34">
         <v>28</v>
       </c>
-      <c r="B35" s="73" t="s">
+      <c r="B35" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="C35" s="73" t="s">
+      <c r="C35" s="38" t="s">
         <v>88</v>
       </c>
       <c r="D35" s="4"/>
@@ -3764,7 +3832,9 @@
       <c r="I35" s="32"/>
       <c r="J35" s="36"/>
       <c r="K35" s="36"/>
-      <c r="L35" s="36"/>
+      <c r="L35" s="36" t="s">
+        <v>6</v>
+      </c>
       <c r="M35" s="36"/>
       <c r="N35" s="36"/>
       <c r="O35" s="36"/>
@@ -3824,10 +3894,10 @@
       <c r="A36" s="34">
         <v>29</v>
       </c>
-      <c r="B36" s="73" t="s">
+      <c r="B36" s="38" t="s">
         <v>89</v>
       </c>
-      <c r="C36" s="73" t="s">
+      <c r="C36" s="38" t="s">
         <v>90</v>
       </c>
       <c r="D36" s="6"/>
@@ -3838,7 +3908,9 @@
       <c r="I36" s="32"/>
       <c r="J36" s="36"/>
       <c r="K36" s="36"/>
-      <c r="L36" s="36"/>
+      <c r="L36" s="36" t="s">
+        <v>6</v>
+      </c>
       <c r="M36" s="36"/>
       <c r="N36" s="36"/>
       <c r="O36" s="36"/>
@@ -3898,10 +3970,10 @@
       <c r="A37" s="34">
         <v>30</v>
       </c>
-      <c r="B37" s="73" t="s">
+      <c r="B37" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="C37" s="73" t="s">
+      <c r="C37" s="38" t="s">
         <v>92</v>
       </c>
       <c r="D37" s="4"/>
@@ -3912,7 +3984,9 @@
       <c r="I37" s="32"/>
       <c r="J37" s="35"/>
       <c r="K37" s="36"/>
-      <c r="L37" s="36"/>
+      <c r="L37" s="36" t="s">
+        <v>6</v>
+      </c>
       <c r="M37" s="36"/>
       <c r="N37" s="36"/>
       <c r="O37" s="36"/>
@@ -3972,10 +4046,10 @@
       <c r="A38" s="34">
         <v>31</v>
       </c>
-      <c r="B38" s="73" t="s">
+      <c r="B38" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="C38" s="73" t="s">
+      <c r="C38" s="38" t="s">
         <v>94</v>
       </c>
       <c r="D38" s="6"/>
@@ -3986,7 +4060,9 @@
       <c r="I38" s="32"/>
       <c r="J38" s="36"/>
       <c r="K38" s="36"/>
-      <c r="L38" s="36"/>
+      <c r="L38" s="36" t="s">
+        <v>6</v>
+      </c>
       <c r="M38" s="36"/>
       <c r="N38" s="36"/>
       <c r="O38" s="36"/>
@@ -4046,10 +4122,10 @@
       <c r="A39" s="34">
         <v>32</v>
       </c>
-      <c r="B39" s="73" t="s">
+      <c r="B39" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="C39" s="73" t="s">
+      <c r="C39" s="38" t="s">
         <v>96</v>
       </c>
       <c r="D39" s="4"/>
@@ -4060,7 +4136,9 @@
       <c r="I39" s="32"/>
       <c r="J39" s="36"/>
       <c r="K39" s="36"/>
-      <c r="L39" s="36"/>
+      <c r="L39" s="36" t="s">
+        <v>6</v>
+      </c>
       <c r="M39" s="36"/>
       <c r="N39" s="36"/>
       <c r="O39" s="36"/>
@@ -4120,10 +4198,10 @@
       <c r="A40" s="34">
         <v>33</v>
       </c>
-      <c r="B40" s="73" t="s">
+      <c r="B40" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="C40" s="73" t="s">
+      <c r="C40" s="38" t="s">
         <v>98</v>
       </c>
       <c r="D40" s="4"/>
@@ -4134,7 +4212,9 @@
       <c r="I40" s="32"/>
       <c r="J40" s="36"/>
       <c r="K40" s="36"/>
-      <c r="L40" s="36"/>
+      <c r="L40" s="36" t="s">
+        <v>6</v>
+      </c>
       <c r="M40" s="36"/>
       <c r="N40" s="35"/>
       <c r="O40" s="36"/>
@@ -4194,10 +4274,10 @@
       <c r="A41" s="34">
         <v>34</v>
       </c>
-      <c r="B41" s="73" t="s">
+      <c r="B41" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="C41" s="73" t="s">
+      <c r="C41" s="38" t="s">
         <v>100</v>
       </c>
       <c r="D41" s="4"/>
@@ -4208,7 +4288,9 @@
       <c r="I41" s="32"/>
       <c r="J41" s="35"/>
       <c r="K41" s="36"/>
-      <c r="L41" s="36"/>
+      <c r="L41" s="36" t="s">
+        <v>6</v>
+      </c>
       <c r="M41" s="36"/>
       <c r="N41" s="36"/>
       <c r="O41" s="36"/>
@@ -4268,10 +4350,10 @@
       <c r="A42" s="34">
         <v>35</v>
       </c>
-      <c r="B42" s="73" t="s">
+      <c r="B42" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="C42" s="73" t="s">
+      <c r="C42" s="38" t="s">
         <v>102</v>
       </c>
       <c r="D42" s="4"/>
@@ -4282,7 +4364,9 @@
       <c r="I42" s="32"/>
       <c r="J42" s="35"/>
       <c r="K42" s="36"/>
-      <c r="L42" s="36"/>
+      <c r="L42" s="36" t="s">
+        <v>6</v>
+      </c>
       <c r="M42" s="36"/>
       <c r="N42" s="36"/>
       <c r="O42" s="36"/>
@@ -4342,10 +4426,10 @@
       <c r="A43" s="34">
         <v>36</v>
       </c>
-      <c r="B43" s="73" t="s">
+      <c r="B43" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="C43" s="73" t="s">
+      <c r="C43" s="38" t="s">
         <v>104</v>
       </c>
       <c r="D43" s="4"/>
@@ -4356,7 +4440,9 @@
       <c r="I43" s="32"/>
       <c r="J43" s="36"/>
       <c r="K43" s="36"/>
-      <c r="L43" s="36"/>
+      <c r="L43" s="36" t="s">
+        <v>6</v>
+      </c>
       <c r="M43" s="36"/>
       <c r="N43" s="36"/>
       <c r="O43" s="36"/>
@@ -4416,10 +4502,10 @@
       <c r="A44" s="34">
         <v>37</v>
       </c>
-      <c r="B44" s="73" t="s">
+      <c r="B44" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="C44" s="73" t="s">
+      <c r="C44" s="38" t="s">
         <v>106</v>
       </c>
       <c r="D44" s="6"/>
@@ -4430,7 +4516,9 @@
       <c r="I44" s="32"/>
       <c r="J44" s="36"/>
       <c r="K44" s="36"/>
-      <c r="L44" s="36"/>
+      <c r="L44" s="36" t="s">
+        <v>6</v>
+      </c>
       <c r="M44" s="35"/>
       <c r="N44" s="35"/>
       <c r="O44" s="36"/>
@@ -4490,10 +4578,10 @@
       <c r="A45" s="34">
         <v>38</v>
       </c>
-      <c r="B45" s="73" t="s">
+      <c r="B45" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="C45" s="73" t="s">
+      <c r="C45" s="38" t="s">
         <v>108</v>
       </c>
       <c r="D45" s="4"/>
@@ -4504,7 +4592,9 @@
       <c r="I45" s="32"/>
       <c r="J45" s="36"/>
       <c r="K45" s="36"/>
-      <c r="L45" s="36"/>
+      <c r="L45" s="36" t="s">
+        <v>6</v>
+      </c>
       <c r="M45" s="36"/>
       <c r="N45" s="35"/>
       <c r="O45" s="36"/>
@@ -4564,10 +4654,10 @@
       <c r="A46" s="34">
         <v>39</v>
       </c>
-      <c r="B46" s="73" t="s">
+      <c r="B46" s="38" t="s">
         <v>109</v>
       </c>
-      <c r="C46" s="73" t="s">
+      <c r="C46" s="38" t="s">
         <v>110</v>
       </c>
       <c r="D46" s="4"/>
@@ -4578,7 +4668,9 @@
       <c r="I46" s="34"/>
       <c r="J46" s="36"/>
       <c r="K46" s="36"/>
-      <c r="L46" s="36"/>
+      <c r="L46" s="36" t="s">
+        <v>6</v>
+      </c>
       <c r="M46" s="36"/>
       <c r="N46" s="35"/>
       <c r="O46" s="36"/>
@@ -4638,10 +4730,10 @@
       <c r="A47" s="34">
         <v>40</v>
       </c>
-      <c r="B47" s="73" t="s">
+      <c r="B47" s="38" t="s">
         <v>111</v>
       </c>
-      <c r="C47" s="73" t="s">
+      <c r="C47" s="38" t="s">
         <v>112</v>
       </c>
       <c r="D47" s="4"/>
@@ -4652,7 +4744,9 @@
       <c r="I47" s="34"/>
       <c r="J47" s="36"/>
       <c r="K47" s="36"/>
-      <c r="L47" s="36"/>
+      <c r="L47" s="36" t="s">
+        <v>6</v>
+      </c>
       <c r="M47" s="36"/>
       <c r="N47" s="35"/>
       <c r="O47" s="36"/>
@@ -4712,10 +4806,10 @@
       <c r="A48" s="34">
         <v>41</v>
       </c>
-      <c r="B48" s="73" t="s">
+      <c r="B48" s="38" t="s">
         <v>113</v>
       </c>
-      <c r="C48" s="73" t="s">
+      <c r="C48" s="38" t="s">
         <v>114</v>
       </c>
       <c r="D48" s="4"/>
@@ -4726,7 +4820,9 @@
       <c r="I48" s="34"/>
       <c r="J48" s="36"/>
       <c r="K48" s="36"/>
-      <c r="L48" s="36"/>
+      <c r="L48" s="36" t="s">
+        <v>6</v>
+      </c>
       <c r="M48" s="36"/>
       <c r="N48" s="35"/>
       <c r="O48" s="36"/>
@@ -4786,10 +4882,10 @@
       <c r="A49" s="34">
         <v>42</v>
       </c>
-      <c r="B49" s="73" t="s">
+      <c r="B49" s="38" t="s">
         <v>115</v>
       </c>
-      <c r="C49" s="73" t="s">
+      <c r="C49" s="38" t="s">
         <v>116</v>
       </c>
       <c r="D49" s="4"/>
@@ -4800,7 +4896,9 @@
       <c r="I49" s="34"/>
       <c r="J49" s="36"/>
       <c r="K49" s="36"/>
-      <c r="L49" s="36"/>
+      <c r="L49" s="36" t="s">
+        <v>6</v>
+      </c>
       <c r="M49" s="36"/>
       <c r="N49" s="35"/>
       <c r="O49" s="36"/>
@@ -4860,10 +4958,10 @@
       <c r="A50" s="34">
         <v>43</v>
       </c>
-      <c r="B50" s="73" t="s">
+      <c r="B50" s="38" t="s">
         <v>117</v>
       </c>
-      <c r="C50" s="73" t="s">
+      <c r="C50" s="38" t="s">
         <v>118</v>
       </c>
       <c r="D50" s="4"/>
@@ -4874,7 +4972,9 @@
       <c r="I50" s="34"/>
       <c r="J50" s="36"/>
       <c r="K50" s="36"/>
-      <c r="L50" s="36"/>
+      <c r="L50" s="36" t="s">
+        <v>6</v>
+      </c>
       <c r="M50" s="36"/>
       <c r="N50" s="35"/>
       <c r="O50" s="36"/>
@@ -4931,174 +5031,174 @@
       <c r="BN50" s="36"/>
     </row>
     <row r="51" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A51" s="69" t="s">
+      <c r="A51" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="B51" s="69"/>
-      <c r="C51" s="70"/>
+      <c r="B51" s="50"/>
+      <c r="C51" s="51"/>
       <c r="D51" s="13"/>
       <c r="E51" s="12">
-        <f>COUNTIF(E8:E50,"A")</f>
+        <f t="shared" ref="E51:AS51" si="0">COUNTIF(E8:E50,"A")</f>
         <v>0</v>
       </c>
       <c r="F51" s="12">
-        <f>COUNTIF(F8:F50,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G51" s="12">
-        <f>COUNTIF(G8:G50,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H51" s="12">
-        <f>COUNTIF(H8:H50,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I51" s="12">
-        <f>COUNTIF(I8:I50,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J51" s="12">
-        <f>COUNTIF(J8:J50,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K51" s="12">
-        <f>COUNTIF(K8:K50,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L51" s="12">
-        <f>COUNTIF(L8:L50,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M51" s="12">
-        <f>COUNTIF(M8:M50,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N51" s="12">
-        <f>COUNTIF(N8:N50,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O51" s="12">
-        <f>COUNTIF(O8:O50,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P51" s="12">
-        <f>COUNTIF(P8:P50,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q51" s="12">
-        <f>COUNTIF(Q8:Q50,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R51" s="12">
-        <f>COUNTIF(R8:R50,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S51" s="12">
-        <f>COUNTIF(S8:S50,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="T51" s="16">
-        <f>COUNTIF(T8:T50,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="U51" s="20">
-        <f>COUNTIF(U8:U50,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="V51" s="20">
-        <f>COUNTIF(V8:V50,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="W51" s="16">
-        <f>COUNTIF(W8:W50,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="X51" s="18">
-        <f>COUNTIF(X8:X50,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Y51" s="16">
-        <f>COUNTIF(Y8:Y50,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Z51" s="12">
-        <f>COUNTIF(Z8:Z50,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AA51" s="12">
-        <f>COUNTIF(AA8:AA50,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AB51" s="12">
-        <f>COUNTIF(AB8:AB50,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AC51" s="12">
-        <f>COUNTIF(AC8:AC50,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AD51" s="12">
-        <f>COUNTIF(AD8:AD50,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AE51" s="12">
-        <f>COUNTIF(AE8:AE50,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AF51" s="12">
-        <f>COUNTIF(AF8:AF50,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AG51" s="12">
-        <f>COUNTIF(AG8:AG50,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AH51" s="12">
-        <f>COUNTIF(AH8:AH50,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AI51" s="27">
-        <f>COUNTIF(AI8:AI50,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AJ51" s="27">
-        <f>COUNTIF(AJ8:AJ50,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AK51" s="27">
-        <f>COUNTIF(AK8:AK50,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AL51" s="27">
-        <f>COUNTIF(AL8:AL50,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AM51" s="27">
-        <f>COUNTIF(AM8:AM50,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AN51" s="27">
-        <f>COUNTIF(AN8:AN50,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AO51" s="27">
-        <f>COUNTIF(AO8:AO50,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AP51" s="27">
-        <f>COUNTIF(AP8:AP50,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AQ51" s="27">
-        <f>COUNTIF(AQ8:AQ50,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AR51" s="27">
-        <f>COUNTIF(AR8:AR50,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AS51" s="30">
-        <f>COUNTIF(AS8:AS50,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AT51" s="30">
@@ -5122,334 +5222,332 @@
         <v>0</v>
       </c>
       <c r="AY51" s="27">
-        <f>COUNTIF(AY8:AY50,"A")</f>
+        <f t="shared" ref="AY51:BN51" si="1">COUNTIF(AY8:AY50,"A")</f>
         <v>0</v>
       </c>
       <c r="AZ51" s="27">
-        <f>COUNTIF(AZ8:AZ50,"A")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BA51" s="27">
-        <f>COUNTIF(BA8:BA50,"A")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BB51" s="27">
-        <f>COUNTIF(BB8:BB50,"A")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BC51" s="27">
-        <f>COUNTIF(BC8:BC50,"A")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BD51" s="27">
-        <f>COUNTIF(BD8:BD50,"A")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BE51" s="27">
-        <f>COUNTIF(BE8:BE50,"A")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BF51" s="27">
-        <f>COUNTIF(BF8:BF50,"A")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BG51" s="27">
-        <f>COUNTIF(BG8:BG50,"A")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BH51" s="27">
-        <f>COUNTIF(BH8:BH50,"A")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BI51" s="27">
-        <f>COUNTIF(BI8:BI50,"A")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BJ51" s="27">
-        <f>COUNTIF(BJ8:BJ50,"A")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BK51" s="27">
-        <f>COUNTIF(BK8:BK50,"A")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BL51" s="27">
-        <f>COUNTIF(BL8:BL50,"A")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BM51" s="27">
-        <f>COUNTIF(BM8:BM50,"A")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BN51" s="27">
-        <f>COUNTIF(BN8:BN50,"A")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A52" s="71" t="s">
+      <c r="A52" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="B52" s="71"/>
-      <c r="C52" s="72"/>
+      <c r="B52" s="40"/>
+      <c r="C52" s="41"/>
       <c r="D52" s="13"/>
       <c r="E52" s="12">
         <f>(43-E51)</f>
         <v>43</v>
       </c>
       <c r="F52" s="34">
-        <f t="shared" ref="F52:BN52" si="0">(43-F51)</f>
+        <f t="shared" ref="F52:BN52" si="2">(43-F51)</f>
         <v>43</v>
       </c>
       <c r="G52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="H52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="I52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="J52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="K52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="L52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="M52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="N52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="O52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="P52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="Q52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="R52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="S52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="T52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="U52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="V52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="W52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="X52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="Y52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="Z52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="AA52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="AB52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="AC52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="AD52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="AE52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="AF52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="AG52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="AH52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="AI52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="AJ52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="AK52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="AL52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="AM52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="AN52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="AO52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="AP52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="AQ52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="AR52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="AS52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="AT52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="AU52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="AV52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="AW52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="AX52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="AY52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="AZ52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="BA52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="BB52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="BC52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="BD52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="BE52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="BF52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="BG52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="BH52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="BI52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="BJ52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="BK52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="BL52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="BM52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="BN52" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A52:C52"/>
-    <mergeCell ref="Y4:AT4"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="A51:C51"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:D4"/>
     <mergeCell ref="G1:J1"/>
     <mergeCell ref="G3:J3"/>
     <mergeCell ref="E4:X4"/>
@@ -5459,17 +5557,19 @@
     <mergeCell ref="O2:X2"/>
     <mergeCell ref="O3:X3"/>
     <mergeCell ref="O1:X1"/>
+    <mergeCell ref="A52:C52"/>
+    <mergeCell ref="Y4:AT4"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="A51:C51"/>
     <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A4:D4"/>
   </mergeCells>
   <conditionalFormatting sqref="E8:BN50">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"OD"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"A"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5482,13 +5582,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" style="68" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" style="37" customWidth="1"/>
     <col min="2" max="2" width="36.28515625" style="1" customWidth="1"/>
     <col min="3" max="5" width="11.140625" style="2" customWidth="1"/>
     <col min="6" max="7" width="11.140625" style="1" customWidth="1"/>
@@ -5498,68 +5598,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="65" t="s">
+      <c r="B1" s="71"/>
+      <c r="C1" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="65"/>
-      <c r="E1" s="66" t="s">
+      <c r="D1" s="55"/>
+      <c r="E1" s="67" t="s">
         <v>121</v>
       </c>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
     </row>
     <row r="2" spans="1:7" ht="19.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="65" t="s">
+      <c r="B2" s="65"/>
+      <c r="C2" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="65"/>
-      <c r="E2" s="66" t="s">
+      <c r="D2" s="55"/>
+      <c r="E2" s="67" t="s">
         <v>120</v>
       </c>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
     </row>
     <row r="3" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="64"/>
-      <c r="C3" s="65" t="s">
+      <c r="B3" s="66"/>
+      <c r="C3" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="65"/>
-      <c r="E3" s="66" t="s">
+      <c r="D3" s="55"/>
+      <c r="E3" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="59" t="s">
+      <c r="A4" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="55" t="s">
+      <c r="B4" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="62" t="s">
+      <c r="C4" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="62"/>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="62"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="60"/>
-      <c r="B5" s="56"/>
+      <c r="A5" s="73"/>
+      <c r="B5" s="47"/>
       <c r="C5" s="21" t="s">
         <v>14</v>
       </c>
@@ -5577,8 +5677,8 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="61"/>
-      <c r="B6" s="57"/>
+      <c r="A6" s="74"/>
+      <c r="B6" s="48"/>
       <c r="C6" s="21">
         <v>50</v>
       </c>
@@ -5596,10 +5696,10 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="74" t="s">
+      <c r="A7" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="73" t="s">
+      <c r="B7" s="38" t="s">
         <v>34</v>
       </c>
       <c r="C7" s="15"/>
@@ -5609,10 +5709,10 @@
       <c r="G7" s="20"/>
     </row>
     <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="74" t="s">
+      <c r="A8" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="73" t="s">
+      <c r="B8" s="38" t="s">
         <v>36</v>
       </c>
       <c r="C8" s="15"/>
@@ -5622,10 +5722,10 @@
       <c r="G8" s="22"/>
     </row>
     <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="74" t="s">
+      <c r="A9" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="73" t="s">
+      <c r="B9" s="38" t="s">
         <v>38</v>
       </c>
       <c r="C9" s="15"/>
@@ -5635,10 +5735,10 @@
       <c r="G9" s="20"/>
     </row>
     <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="74" t="s">
+      <c r="A10" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="73" t="s">
+      <c r="B10" s="38" t="s">
         <v>40</v>
       </c>
       <c r="C10" s="15"/>
@@ -5648,10 +5748,10 @@
       <c r="G10" s="20"/>
     </row>
     <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="74" t="s">
+      <c r="A11" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="73" t="s">
+      <c r="B11" s="38" t="s">
         <v>42</v>
       </c>
       <c r="C11" s="15"/>
@@ -5661,10 +5761,10 @@
       <c r="G11" s="20"/>
     </row>
     <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="74" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" s="73" t="s">
+      <c r="A12" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="38" t="s">
         <v>44</v>
       </c>
       <c r="C12" s="15"/>
@@ -5674,10 +5774,10 @@
       <c r="G12" s="20"/>
     </row>
     <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="74" t="s">
+      <c r="A13" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="73" t="s">
+      <c r="B13" s="38" t="s">
         <v>46</v>
       </c>
       <c r="C13" s="15"/>
@@ -5687,10 +5787,10 @@
       <c r="G13" s="20"/>
     </row>
     <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="74" t="s">
+      <c r="A14" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="73" t="s">
+      <c r="B14" s="38" t="s">
         <v>48</v>
       </c>
       <c r="C14" s="15"/>
@@ -5700,10 +5800,10 @@
       <c r="G14" s="20"/>
     </row>
     <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="74" t="s">
+      <c r="A15" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="73" t="s">
+      <c r="B15" s="38" t="s">
         <v>50</v>
       </c>
       <c r="C15" s="15"/>
@@ -5713,10 +5813,10 @@
       <c r="G15" s="20"/>
     </row>
     <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="74" t="s">
+      <c r="A16" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="73" t="s">
+      <c r="B16" s="38" t="s">
         <v>52</v>
       </c>
       <c r="C16" s="15"/>
@@ -5726,10 +5826,10 @@
       <c r="G16" s="20"/>
     </row>
     <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="74" t="s">
+      <c r="A17" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="73" t="s">
+      <c r="B17" s="38" t="s">
         <v>54</v>
       </c>
       <c r="C17" s="15"/>
@@ -5739,10 +5839,10 @@
       <c r="G17" s="20"/>
     </row>
     <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="74" t="s">
+      <c r="A18" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="B18" s="73" t="s">
+      <c r="B18" s="38" t="s">
         <v>56</v>
       </c>
       <c r="C18" s="15"/>
@@ -5752,10 +5852,10 @@
       <c r="G18" s="20"/>
     </row>
     <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="74" t="s">
+      <c r="A19" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="73" t="s">
+      <c r="B19" s="38" t="s">
         <v>58</v>
       </c>
       <c r="C19" s="15"/>
@@ -5765,10 +5865,10 @@
       <c r="G19" s="20"/>
     </row>
     <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="74" t="s">
+      <c r="A20" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="B20" s="73" t="s">
+      <c r="B20" s="38" t="s">
         <v>60</v>
       </c>
       <c r="C20" s="15"/>
@@ -5778,10 +5878,10 @@
       <c r="G20" s="20"/>
     </row>
     <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="74" t="s">
+      <c r="A21" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="B21" s="73" t="s">
+      <c r="B21" s="38" t="s">
         <v>62</v>
       </c>
       <c r="C21" s="15"/>
@@ -5791,10 +5891,10 @@
       <c r="G21" s="20"/>
     </row>
     <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="74" t="s">
+      <c r="A22" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="B22" s="73" t="s">
+      <c r="B22" s="38" t="s">
         <v>64</v>
       </c>
       <c r="C22" s="15"/>
@@ -5804,10 +5904,10 @@
       <c r="G22" s="20"/>
     </row>
     <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="74" t="s">
+      <c r="A23" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="B23" s="73" t="s">
+      <c r="B23" s="38" t="s">
         <v>66</v>
       </c>
       <c r="C23" s="15"/>
@@ -5817,10 +5917,10 @@
       <c r="G23" s="22"/>
     </row>
     <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="74" t="s">
+      <c r="A24" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="B24" s="73" t="s">
+      <c r="B24" s="38" t="s">
         <v>68</v>
       </c>
       <c r="C24" s="15"/>
@@ -5830,10 +5930,10 @@
       <c r="G24" s="20"/>
     </row>
     <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="74" t="s">
+      <c r="A25" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="B25" s="73" t="s">
+      <c r="B25" s="38" t="s">
         <v>70</v>
       </c>
       <c r="C25" s="15"/>
@@ -5843,10 +5943,10 @@
       <c r="G25" s="20"/>
     </row>
     <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="74" t="s">
+      <c r="A26" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="B26" s="73" t="s">
+      <c r="B26" s="38" t="s">
         <v>72</v>
       </c>
       <c r="C26" s="15"/>
@@ -5856,10 +5956,10 @@
       <c r="G26" s="20"/>
     </row>
     <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="74" t="s">
+      <c r="A27" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="B27" s="73" t="s">
+      <c r="B27" s="38" t="s">
         <v>74</v>
       </c>
       <c r="C27" s="15"/>
@@ -5869,10 +5969,10 @@
       <c r="G27" s="20"/>
     </row>
     <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="74" t="s">
+      <c r="A28" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="B28" s="73" t="s">
+      <c r="B28" s="38" t="s">
         <v>76</v>
       </c>
       <c r="C28" s="15"/>
@@ -5882,10 +5982,10 @@
       <c r="G28" s="20"/>
     </row>
     <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="74" t="s">
+      <c r="A29" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="B29" s="73" t="s">
+      <c r="B29" s="38" t="s">
         <v>78</v>
       </c>
       <c r="C29" s="15"/>
@@ -5895,10 +5995,10 @@
       <c r="G29" s="20"/>
     </row>
     <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="74" t="s">
+      <c r="A30" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="B30" s="73" t="s">
+      <c r="B30" s="38" t="s">
         <v>80</v>
       </c>
       <c r="C30" s="15"/>
@@ -5908,10 +6008,10 @@
       <c r="G30" s="20"/>
     </row>
     <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="74" t="s">
+      <c r="A31" s="39" t="s">
         <v>81</v>
       </c>
-      <c r="B31" s="73" t="s">
+      <c r="B31" s="38" t="s">
         <v>82</v>
       </c>
       <c r="C31" s="15"/>
@@ -5921,10 +6021,10 @@
       <c r="G31" s="20"/>
     </row>
     <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="74" t="s">
+      <c r="A32" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="B32" s="73" t="s">
+      <c r="B32" s="38" t="s">
         <v>84</v>
       </c>
       <c r="C32" s="15"/>
@@ -5934,10 +6034,10 @@
       <c r="G32" s="20"/>
     </row>
     <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="74" t="s">
+      <c r="A33" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="B33" s="73" t="s">
+      <c r="B33" s="38" t="s">
         <v>86</v>
       </c>
       <c r="C33" s="15"/>
@@ -5947,10 +6047,10 @@
       <c r="G33" s="20"/>
     </row>
     <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="74" t="s">
+      <c r="A34" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="B34" s="73" t="s">
+      <c r="B34" s="38" t="s">
         <v>88</v>
       </c>
       <c r="C34" s="15"/>
@@ -5960,10 +6060,10 @@
       <c r="G34" s="20"/>
     </row>
     <row r="35" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="74" t="s">
+      <c r="A35" s="39" t="s">
         <v>89</v>
       </c>
-      <c r="B35" s="73" t="s">
+      <c r="B35" s="38" t="s">
         <v>90</v>
       </c>
       <c r="C35" s="15"/>
@@ -5973,10 +6073,10 @@
       <c r="G35" s="20"/>
     </row>
     <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="74" t="s">
+      <c r="A36" s="39" t="s">
         <v>91</v>
       </c>
-      <c r="B36" s="73" t="s">
+      <c r="B36" s="38" t="s">
         <v>92</v>
       </c>
       <c r="C36" s="15"/>
@@ -5986,10 +6086,10 @@
       <c r="G36" s="20"/>
     </row>
     <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="74" t="s">
+      <c r="A37" s="39" t="s">
         <v>93</v>
       </c>
-      <c r="B37" s="73" t="s">
+      <c r="B37" s="38" t="s">
         <v>94</v>
       </c>
       <c r="C37" s="15"/>
@@ -5999,10 +6099,10 @@
       <c r="G37" s="20"/>
     </row>
     <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="74" t="s">
+      <c r="A38" s="39" t="s">
         <v>95</v>
       </c>
-      <c r="B38" s="73" t="s">
+      <c r="B38" s="38" t="s">
         <v>96</v>
       </c>
       <c r="C38" s="15"/>
@@ -6012,10 +6112,10 @@
       <c r="G38" s="20"/>
     </row>
     <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="74" t="s">
+      <c r="A39" s="39" t="s">
         <v>97</v>
       </c>
-      <c r="B39" s="73" t="s">
+      <c r="B39" s="38" t="s">
         <v>98</v>
       </c>
       <c r="C39" s="15"/>
@@ -6025,10 +6125,10 @@
       <c r="G39" s="20"/>
     </row>
     <row r="40" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="74" t="s">
+      <c r="A40" s="39" t="s">
         <v>99</v>
       </c>
-      <c r="B40" s="73" t="s">
+      <c r="B40" s="38" t="s">
         <v>100</v>
       </c>
       <c r="C40" s="15"/>
@@ -6038,10 +6138,10 @@
       <c r="G40" s="20"/>
     </row>
     <row r="41" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="74" t="s">
+      <c r="A41" s="39" t="s">
         <v>101</v>
       </c>
-      <c r="B41" s="73" t="s">
+      <c r="B41" s="38" t="s">
         <v>102</v>
       </c>
       <c r="C41" s="15"/>
@@ -6051,10 +6151,10 @@
       <c r="G41" s="20"/>
     </row>
     <row r="42" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="74" t="s">
+      <c r="A42" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="B42" s="73" t="s">
+      <c r="B42" s="38" t="s">
         <v>104</v>
       </c>
       <c r="C42" s="15"/>
@@ -6064,10 +6164,10 @@
       <c r="G42" s="20"/>
     </row>
     <row r="43" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="74" t="s">
+      <c r="A43" s="39" t="s">
         <v>105</v>
       </c>
-      <c r="B43" s="73" t="s">
+      <c r="B43" s="38" t="s">
         <v>106</v>
       </c>
       <c r="C43" s="15"/>
@@ -6077,10 +6177,10 @@
       <c r="G43" s="20"/>
     </row>
     <row r="44" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="74" t="s">
+      <c r="A44" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="B44" s="73" t="s">
+      <c r="B44" s="38" t="s">
         <v>108</v>
       </c>
       <c r="C44" s="15"/>
@@ -6090,10 +6190,10 @@
       <c r="G44" s="20"/>
     </row>
     <row r="45" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="74" t="s">
+      <c r="A45" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="B45" s="73" t="s">
+      <c r="B45" s="38" t="s">
         <v>110</v>
       </c>
       <c r="C45" s="34"/>
@@ -6103,10 +6203,10 @@
       <c r="G45" s="34"/>
     </row>
     <row r="46" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="74" t="s">
+      <c r="A46" s="39" t="s">
         <v>111</v>
       </c>
-      <c r="B46" s="73" t="s">
+      <c r="B46" s="38" t="s">
         <v>112</v>
       </c>
       <c r="C46" s="34"/>
@@ -6116,10 +6216,10 @@
       <c r="G46" s="34"/>
     </row>
     <row r="47" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="74" t="s">
+      <c r="A47" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="B47" s="73" t="s">
+      <c r="B47" s="38" t="s">
         <v>114</v>
       </c>
       <c r="C47" s="34"/>
@@ -6129,10 +6229,10 @@
       <c r="G47" s="34"/>
     </row>
     <row r="48" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="74" t="s">
+      <c r="A48" s="39" t="s">
         <v>115</v>
       </c>
-      <c r="B48" s="73" t="s">
+      <c r="B48" s="38" t="s">
         <v>116</v>
       </c>
       <c r="C48" s="15"/>
@@ -6142,10 +6242,10 @@
       <c r="G48" s="20"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="74" t="s">
+      <c r="A49" s="39" t="s">
         <v>117</v>
       </c>
-      <c r="B49" s="73" t="s">
+      <c r="B49" s="38" t="s">
         <v>118</v>
       </c>
       <c r="C49" s="34"/>
@@ -6155,10 +6255,10 @@
       <c r="G49" s="34"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="53" t="s">
+      <c r="A50" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="B50" s="54"/>
+      <c r="B50" s="70"/>
       <c r="C50" s="16"/>
       <c r="D50" s="16"/>
       <c r="E50" s="20"/>
@@ -6166,10 +6266,10 @@
       <c r="G50" s="13"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="53" t="s">
+      <c r="A51" s="69" t="s">
         <v>16</v>
       </c>
-      <c r="B51" s="54"/>
+      <c r="B51" s="70"/>
       <c r="C51" s="16"/>
       <c r="D51" s="16"/>
       <c r="E51" s="20"/>
@@ -6177,10 +6277,10 @@
       <c r="G51" s="13"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="53" t="s">
+      <c r="A52" s="69" t="s">
         <v>17</v>
       </c>
-      <c r="B52" s="54"/>
+      <c r="B52" s="70"/>
       <c r="C52" s="17"/>
       <c r="D52" s="16"/>
       <c r="E52" s="20"/>
@@ -6189,6 +6289,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
     <mergeCell ref="C4:G4"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
@@ -6198,20 +6304,14 @@
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="E3:G3"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:B6"/>
   </mergeCells>
   <conditionalFormatting sqref="C7:G48">
-    <cfRule type="cellIs" dxfId="1" priority="19" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="19" operator="lessThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:G49">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Last Update 05-02-2019 18:00:04.50
</commit_message>
<xml_diff>
--- a/Acadamic Log Book MC-18-19.xlsx
+++ b/Acadamic Log Book MC-18-19.xlsx
@@ -768,45 +768,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="17" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="1" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="1" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -834,6 +795,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -852,14 +816,41 @@
     <xf numFmtId="17" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="17" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="17" fontId="1" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="17" fontId="1" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -878,6 +869,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1277,51 +1277,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:66" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="50"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="38"/>
       <c r="E1" s="17" t="s">
         <v>6</v>
       </c>
       <c r="F1" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="53" t="s">
+      <c r="G1" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="56" t="s">
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56"/>
-      <c r="O1" s="58" t="s">
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="47" t="s">
         <v>117</v>
       </c>
-      <c r="P1" s="59"/>
-      <c r="Q1" s="59"/>
-      <c r="R1" s="59"/>
-      <c r="S1" s="59"/>
-      <c r="T1" s="59"/>
-      <c r="U1" s="59"/>
-      <c r="V1" s="59"/>
-      <c r="W1" s="59"/>
-      <c r="X1" s="60"/>
-      <c r="Y1" s="47" t="s">
+      <c r="P1" s="48"/>
+      <c r="Q1" s="48"/>
+      <c r="R1" s="48"/>
+      <c r="S1" s="48"/>
+      <c r="T1" s="48"/>
+      <c r="U1" s="48"/>
+      <c r="V1" s="48"/>
+      <c r="W1" s="48"/>
+      <c r="X1" s="49"/>
+      <c r="Y1" s="35" t="s">
         <v>119</v>
       </c>
-      <c r="Z1" s="48"/>
-      <c r="AA1" s="48"/>
-      <c r="AB1" s="48"/>
-      <c r="AC1" s="48"/>
-      <c r="AD1" s="48"/>
-      <c r="AE1" s="48"/>
+      <c r="Z1" s="36"/>
+      <c r="AA1" s="36"/>
+      <c r="AB1" s="36"/>
+      <c r="AC1" s="36"/>
+      <c r="AD1" s="36"/>
+      <c r="AE1" s="36"/>
       <c r="AF1" s="2" t="s">
         <v>120</v>
       </c>
@@ -1329,42 +1329,42 @@
       <c r="AH1" s="21"/>
     </row>
     <row r="2" spans="1:66" ht="19.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="52"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="40"/>
       <c r="E2" s="11" t="s">
         <v>8</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="40" t="s">
+      <c r="G2" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="56" t="s">
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="56"/>
-      <c r="M2" s="56"/>
-      <c r="N2" s="56"/>
-      <c r="O2" s="57" t="s">
+      <c r="L2" s="45"/>
+      <c r="M2" s="45"/>
+      <c r="N2" s="45"/>
+      <c r="O2" s="46" t="s">
         <v>116</v>
       </c>
-      <c r="P2" s="57"/>
-      <c r="Q2" s="57"/>
-      <c r="R2" s="57"/>
-      <c r="S2" s="57"/>
-      <c r="T2" s="57"/>
-      <c r="U2" s="57"/>
-      <c r="V2" s="57"/>
-      <c r="W2" s="57"/>
-      <c r="X2" s="57"/>
+      <c r="P2" s="46"/>
+      <c r="Q2" s="46"/>
+      <c r="R2" s="46"/>
+      <c r="S2" s="46"/>
+      <c r="T2" s="46"/>
+      <c r="U2" s="46"/>
+      <c r="V2" s="46"/>
+      <c r="W2" s="46"/>
+      <c r="X2" s="46"/>
       <c r="Y2" s="21"/>
       <c r="Z2" s="21"/>
       <c r="AA2" s="21"/>
@@ -1377,42 +1377,42 @@
       <c r="AH2" s="21"/>
     </row>
     <row r="3" spans="1:66" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="37" t="s">
         <v>118</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="50"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="38"/>
       <c r="E3" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F3" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="40" t="s">
+      <c r="G3" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="56" t="s">
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="56"/>
-      <c r="M3" s="56"/>
-      <c r="N3" s="56"/>
-      <c r="O3" s="57" t="s">
+      <c r="L3" s="45"/>
+      <c r="M3" s="45"/>
+      <c r="N3" s="45"/>
+      <c r="O3" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="P3" s="57"/>
-      <c r="Q3" s="57"/>
-      <c r="R3" s="57"/>
-      <c r="S3" s="57"/>
-      <c r="T3" s="57"/>
-      <c r="U3" s="57"/>
-      <c r="V3" s="57"/>
-      <c r="W3" s="57"/>
-      <c r="X3" s="57"/>
+      <c r="P3" s="46"/>
+      <c r="Q3" s="46"/>
+      <c r="R3" s="46"/>
+      <c r="S3" s="46"/>
+      <c r="T3" s="46"/>
+      <c r="U3" s="46"/>
+      <c r="V3" s="46"/>
+      <c r="W3" s="46"/>
+      <c r="X3" s="46"/>
       <c r="Y3" s="22"/>
       <c r="Z3" s="22"/>
       <c r="AA3" s="22"/>
@@ -1425,58 +1425,58 @@
       <c r="AH3" s="22"/>
     </row>
     <row r="4" spans="1:66" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="61">
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="50">
         <v>43435</v>
       </c>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
-      <c r="H4" s="61"/>
-      <c r="I4" s="61"/>
-      <c r="J4" s="61"/>
-      <c r="K4" s="61"/>
-      <c r="L4" s="61"/>
-      <c r="M4" s="61"/>
-      <c r="N4" s="61"/>
-      <c r="O4" s="61"/>
-      <c r="P4" s="61"/>
-      <c r="Q4" s="37">
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="50"/>
+      <c r="L4" s="50"/>
+      <c r="M4" s="50"/>
+      <c r="N4" s="50"/>
+      <c r="O4" s="50"/>
+      <c r="P4" s="50"/>
+      <c r="Q4" s="51">
         <v>43466</v>
       </c>
-      <c r="R4" s="38"/>
-      <c r="S4" s="38"/>
-      <c r="T4" s="38"/>
-      <c r="U4" s="38"/>
-      <c r="V4" s="38"/>
-      <c r="W4" s="38"/>
-      <c r="X4" s="39"/>
-      <c r="Y4" s="37"/>
-      <c r="Z4" s="38"/>
-      <c r="AA4" s="38"/>
-      <c r="AB4" s="38"/>
-      <c r="AC4" s="38"/>
-      <c r="AD4" s="38"/>
-      <c r="AE4" s="38"/>
-      <c r="AF4" s="38"/>
-      <c r="AG4" s="38"/>
-      <c r="AH4" s="38"/>
-      <c r="AI4" s="38"/>
-      <c r="AJ4" s="38"/>
-      <c r="AK4" s="38"/>
-      <c r="AL4" s="38"/>
-      <c r="AM4" s="38"/>
-      <c r="AN4" s="38"/>
-      <c r="AO4" s="38"/>
-      <c r="AP4" s="38"/>
-      <c r="AQ4" s="38"/>
-      <c r="AR4" s="38"/>
-      <c r="AS4" s="38"/>
-      <c r="AT4" s="39"/>
+      <c r="R4" s="52"/>
+      <c r="S4" s="52"/>
+      <c r="T4" s="52"/>
+      <c r="U4" s="52"/>
+      <c r="V4" s="52"/>
+      <c r="W4" s="52"/>
+      <c r="X4" s="53"/>
+      <c r="Y4" s="51"/>
+      <c r="Z4" s="52"/>
+      <c r="AA4" s="52"/>
+      <c r="AB4" s="52"/>
+      <c r="AC4" s="52"/>
+      <c r="AD4" s="52"/>
+      <c r="AE4" s="52"/>
+      <c r="AF4" s="52"/>
+      <c r="AG4" s="52"/>
+      <c r="AH4" s="52"/>
+      <c r="AI4" s="52"/>
+      <c r="AJ4" s="52"/>
+      <c r="AK4" s="52"/>
+      <c r="AL4" s="52"/>
+      <c r="AM4" s="52"/>
+      <c r="AN4" s="52"/>
+      <c r="AO4" s="52"/>
+      <c r="AP4" s="52"/>
+      <c r="AQ4" s="52"/>
+      <c r="AR4" s="52"/>
+      <c r="AS4" s="52"/>
+      <c r="AT4" s="53"/>
       <c r="AU4" s="23"/>
       <c r="AV4" s="23"/>
       <c r="AW4" s="23"/>
@@ -1499,13 +1499,13 @@
       <c r="BN4" s="23"/>
     </row>
     <row r="5" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="56" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="9" t="s">
@@ -1615,9 +1615,9 @@
       <c r="BN5" s="28"/>
     </row>
     <row r="6" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A6" s="44"/>
-      <c r="B6" s="44"/>
-      <c r="C6" s="42"/>
+      <c r="A6" s="59"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="57"/>
       <c r="D6" s="9" t="s">
         <v>1</v>
       </c>
@@ -1725,11 +1725,11 @@
       <c r="BN6" s="28"/>
     </row>
     <row r="7" spans="1:66" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
+      <c r="A7" s="59"/>
       <c r="B7" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="C7" s="43"/>
+      <c r="C7" s="58"/>
       <c r="D7" s="10" t="s">
         <v>2</v>
       </c>
@@ -6395,11 +6395,11 @@
       <c r="BN50" s="29"/>
     </row>
     <row r="51" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A51" s="45" t="s">
+      <c r="A51" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="B51" s="45"/>
-      <c r="C51" s="46"/>
+      <c r="B51" s="60"/>
+      <c r="C51" s="61"/>
       <c r="D51" s="13"/>
       <c r="E51" s="12">
         <f t="shared" ref="E51:AS51" si="0">COUNTIF(E8:E50,"A")</f>
@@ -6651,11 +6651,11 @@
       </c>
     </row>
     <row r="52" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A52" s="35" t="s">
+      <c r="A52" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="B52" s="35"/>
-      <c r="C52" s="36"/>
+      <c r="B52" s="54"/>
+      <c r="C52" s="55"/>
       <c r="D52" s="13"/>
       <c r="E52" s="12">
         <f>(43-E51)</f>
@@ -6909,6 +6909,13 @@
   </sheetData>
   <autoFilter ref="N1:N52"/>
   <mergeCells count="22">
+    <mergeCell ref="A52:C52"/>
+    <mergeCell ref="Y4:AT4"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="A51:C51"/>
+    <mergeCell ref="A5:A7"/>
     <mergeCell ref="Y1:AE1"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
@@ -6924,13 +6931,6 @@
     <mergeCell ref="O1:X1"/>
     <mergeCell ref="E4:P4"/>
     <mergeCell ref="Q4:X4"/>
-    <mergeCell ref="A52:C52"/>
-    <mergeCell ref="Y4:AT4"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="A51:C51"/>
-    <mergeCell ref="A5:A7"/>
   </mergeCells>
   <conditionalFormatting sqref="E8:S50 U8:BN50">
     <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
@@ -6957,8 +6957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6973,68 +6973,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="56" t="s">
+      <c r="B1" s="64"/>
+      <c r="C1" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="56"/>
-      <c r="E1" s="57" t="s">
+      <c r="D1" s="45"/>
+      <c r="E1" s="46" t="s">
         <v>117</v>
       </c>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
     </row>
     <row r="2" spans="1:7" ht="19.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="56" t="s">
+      <c r="B2" s="69"/>
+      <c r="C2" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="56"/>
-      <c r="E2" s="57" t="s">
+      <c r="D2" s="45"/>
+      <c r="E2" s="46" t="s">
         <v>116</v>
       </c>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
     </row>
     <row r="3" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="70" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="64"/>
-      <c r="C3" s="56" t="s">
+      <c r="B3" s="70"/>
+      <c r="C3" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="56"/>
-      <c r="E3" s="57" t="s">
+      <c r="D3" s="45"/>
+      <c r="E3" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="68" t="s">
+      <c r="A4" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="62" t="s">
+      <c r="C4" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="62"/>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="62"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="68"/>
+      <c r="G4" s="68"/>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="69"/>
-      <c r="B5" s="42"/>
+      <c r="A5" s="66"/>
+      <c r="B5" s="57"/>
       <c r="C5" s="18" t="s">
         <v>14</v>
       </c>
@@ -7048,8 +7048,8 @@
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="70"/>
-      <c r="B6" s="43"/>
+      <c r="A6" s="67"/>
+      <c r="B6" s="58"/>
       <c r="C6" s="18">
         <v>25</v>
       </c>
@@ -7489,13 +7489,15 @@
       <c r="B28" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="C28" s="26"/>
+      <c r="C28" s="26">
+        <v>15</v>
+      </c>
       <c r="D28" s="26">
         <v>65</v>
       </c>
       <c r="E28" s="26">
         <f t="shared" si="0"/>
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="F28" s="26"/>
       <c r="G28" s="26"/>
@@ -7919,10 +7921,10 @@
       <c r="G49" s="26"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="65" t="s">
+      <c r="A50" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="B50" s="66"/>
+      <c r="B50" s="63"/>
       <c r="C50" s="14"/>
       <c r="D50" s="14"/>
       <c r="E50" s="17"/>
@@ -7930,10 +7932,10 @@
       <c r="G50" s="13"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="65" t="s">
+      <c r="A51" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="B51" s="66"/>
+      <c r="B51" s="63"/>
       <c r="C51" s="14"/>
       <c r="D51" s="14"/>
       <c r="E51" s="17"/>
@@ -7941,10 +7943,10 @@
       <c r="G51" s="13"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="65" t="s">
+      <c r="A52" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="B52" s="66"/>
+      <c r="B52" s="63"/>
       <c r="C52" s="15"/>
       <c r="D52" s="14"/>
       <c r="E52" s="17"/>
@@ -7953,12 +7955,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:B6"/>
     <mergeCell ref="C4:G4"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
@@ -7968,6 +7964,12 @@
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="E3:G3"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
   </mergeCells>
   <conditionalFormatting sqref="C7:C49">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">

</xml_diff>

<commit_message>
Last Update 06-02-2019 18:24:32.01
</commit_message>
<xml_diff>
--- a/Acadamic Log Book MC-18-19.xlsx
+++ b/Acadamic Log Book MC-18-19.xlsx
@@ -768,6 +768,45 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="17" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="1" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="1" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -795,9 +834,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -816,41 +852,14 @@
     <xf numFmtId="17" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="17" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="17" fontId="1" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="17" fontId="1" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -869,15 +878,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1277,51 +1277,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:66" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="38"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="50"/>
       <c r="E1" s="17" t="s">
         <v>6</v>
       </c>
       <c r="F1" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="41" t="s">
+      <c r="G1" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="45" t="s">
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="47" t="s">
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="58" t="s">
         <v>117</v>
       </c>
-      <c r="P1" s="48"/>
-      <c r="Q1" s="48"/>
-      <c r="R1" s="48"/>
-      <c r="S1" s="48"/>
-      <c r="T1" s="48"/>
-      <c r="U1" s="48"/>
-      <c r="V1" s="48"/>
-      <c r="W1" s="48"/>
-      <c r="X1" s="49"/>
-      <c r="Y1" s="35" t="s">
+      <c r="P1" s="59"/>
+      <c r="Q1" s="59"/>
+      <c r="R1" s="59"/>
+      <c r="S1" s="59"/>
+      <c r="T1" s="59"/>
+      <c r="U1" s="59"/>
+      <c r="V1" s="59"/>
+      <c r="W1" s="59"/>
+      <c r="X1" s="60"/>
+      <c r="Y1" s="47" t="s">
         <v>119</v>
       </c>
-      <c r="Z1" s="36"/>
-      <c r="AA1" s="36"/>
-      <c r="AB1" s="36"/>
-      <c r="AC1" s="36"/>
-      <c r="AD1" s="36"/>
-      <c r="AE1" s="36"/>
+      <c r="Z1" s="48"/>
+      <c r="AA1" s="48"/>
+      <c r="AB1" s="48"/>
+      <c r="AC1" s="48"/>
+      <c r="AD1" s="48"/>
+      <c r="AE1" s="48"/>
       <c r="AF1" s="2" t="s">
         <v>120</v>
       </c>
@@ -1329,42 +1329,42 @@
       <c r="AH1" s="21"/>
     </row>
     <row r="2" spans="1:66" ht="19.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="40"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="52"/>
       <c r="E2" s="11" t="s">
         <v>8</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="44" t="s">
+      <c r="G2" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="45" t="s">
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="45"/>
-      <c r="M2" s="45"/>
-      <c r="N2" s="45"/>
-      <c r="O2" s="46" t="s">
+      <c r="L2" s="56"/>
+      <c r="M2" s="56"/>
+      <c r="N2" s="56"/>
+      <c r="O2" s="57" t="s">
         <v>116</v>
       </c>
-      <c r="P2" s="46"/>
-      <c r="Q2" s="46"/>
-      <c r="R2" s="46"/>
-      <c r="S2" s="46"/>
-      <c r="T2" s="46"/>
-      <c r="U2" s="46"/>
-      <c r="V2" s="46"/>
-      <c r="W2" s="46"/>
-      <c r="X2" s="46"/>
+      <c r="P2" s="57"/>
+      <c r="Q2" s="57"/>
+      <c r="R2" s="57"/>
+      <c r="S2" s="57"/>
+      <c r="T2" s="57"/>
+      <c r="U2" s="57"/>
+      <c r="V2" s="57"/>
+      <c r="W2" s="57"/>
+      <c r="X2" s="57"/>
       <c r="Y2" s="21"/>
       <c r="Z2" s="21"/>
       <c r="AA2" s="21"/>
@@ -1377,42 +1377,42 @@
       <c r="AH2" s="21"/>
     </row>
     <row r="3" spans="1:66" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="49" t="s">
         <v>118</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="38"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="50"/>
       <c r="E3" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F3" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="44" t="s">
+      <c r="G3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="45" t="s">
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="45"/>
-      <c r="M3" s="45"/>
-      <c r="N3" s="45"/>
-      <c r="O3" s="46" t="s">
+      <c r="L3" s="56"/>
+      <c r="M3" s="56"/>
+      <c r="N3" s="56"/>
+      <c r="O3" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="P3" s="46"/>
-      <c r="Q3" s="46"/>
-      <c r="R3" s="46"/>
-      <c r="S3" s="46"/>
-      <c r="T3" s="46"/>
-      <c r="U3" s="46"/>
-      <c r="V3" s="46"/>
-      <c r="W3" s="46"/>
-      <c r="X3" s="46"/>
+      <c r="P3" s="57"/>
+      <c r="Q3" s="57"/>
+      <c r="R3" s="57"/>
+      <c r="S3" s="57"/>
+      <c r="T3" s="57"/>
+      <c r="U3" s="57"/>
+      <c r="V3" s="57"/>
+      <c r="W3" s="57"/>
+      <c r="X3" s="57"/>
       <c r="Y3" s="22"/>
       <c r="Z3" s="22"/>
       <c r="AA3" s="22"/>
@@ -1425,58 +1425,58 @@
       <c r="AH3" s="22"/>
     </row>
     <row r="4" spans="1:66" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="50">
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="61">
         <v>43435</v>
       </c>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
-      <c r="H4" s="50"/>
-      <c r="I4" s="50"/>
-      <c r="J4" s="50"/>
-      <c r="K4" s="50"/>
-      <c r="L4" s="50"/>
-      <c r="M4" s="50"/>
-      <c r="N4" s="50"/>
-      <c r="O4" s="50"/>
-      <c r="P4" s="50"/>
-      <c r="Q4" s="51">
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="61"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="61"/>
+      <c r="L4" s="61"/>
+      <c r="M4" s="61"/>
+      <c r="N4" s="61"/>
+      <c r="O4" s="61"/>
+      <c r="P4" s="61"/>
+      <c r="Q4" s="37">
         <v>43466</v>
       </c>
-      <c r="R4" s="52"/>
-      <c r="S4" s="52"/>
-      <c r="T4" s="52"/>
-      <c r="U4" s="52"/>
-      <c r="V4" s="52"/>
-      <c r="W4" s="52"/>
-      <c r="X4" s="53"/>
-      <c r="Y4" s="51"/>
-      <c r="Z4" s="52"/>
-      <c r="AA4" s="52"/>
-      <c r="AB4" s="52"/>
-      <c r="AC4" s="52"/>
-      <c r="AD4" s="52"/>
-      <c r="AE4" s="52"/>
-      <c r="AF4" s="52"/>
-      <c r="AG4" s="52"/>
-      <c r="AH4" s="52"/>
-      <c r="AI4" s="52"/>
-      <c r="AJ4" s="52"/>
-      <c r="AK4" s="52"/>
-      <c r="AL4" s="52"/>
-      <c r="AM4" s="52"/>
-      <c r="AN4" s="52"/>
-      <c r="AO4" s="52"/>
-      <c r="AP4" s="52"/>
-      <c r="AQ4" s="52"/>
-      <c r="AR4" s="52"/>
-      <c r="AS4" s="52"/>
-      <c r="AT4" s="53"/>
+      <c r="R4" s="38"/>
+      <c r="S4" s="38"/>
+      <c r="T4" s="38"/>
+      <c r="U4" s="38"/>
+      <c r="V4" s="38"/>
+      <c r="W4" s="38"/>
+      <c r="X4" s="39"/>
+      <c r="Y4" s="37"/>
+      <c r="Z4" s="38"/>
+      <c r="AA4" s="38"/>
+      <c r="AB4" s="38"/>
+      <c r="AC4" s="38"/>
+      <c r="AD4" s="38"/>
+      <c r="AE4" s="38"/>
+      <c r="AF4" s="38"/>
+      <c r="AG4" s="38"/>
+      <c r="AH4" s="38"/>
+      <c r="AI4" s="38"/>
+      <c r="AJ4" s="38"/>
+      <c r="AK4" s="38"/>
+      <c r="AL4" s="38"/>
+      <c r="AM4" s="38"/>
+      <c r="AN4" s="38"/>
+      <c r="AO4" s="38"/>
+      <c r="AP4" s="38"/>
+      <c r="AQ4" s="38"/>
+      <c r="AR4" s="38"/>
+      <c r="AS4" s="38"/>
+      <c r="AT4" s="39"/>
       <c r="AU4" s="23"/>
       <c r="AV4" s="23"/>
       <c r="AW4" s="23"/>
@@ -1499,13 +1499,13 @@
       <c r="BN4" s="23"/>
     </row>
     <row r="5" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A5" s="59" t="s">
+      <c r="A5" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="56" t="s">
+      <c r="C5" s="41" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="9" t="s">
@@ -1615,9 +1615,9 @@
       <c r="BN5" s="28"/>
     </row>
     <row r="6" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A6" s="59"/>
-      <c r="B6" s="59"/>
-      <c r="C6" s="57"/>
+      <c r="A6" s="44"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="42"/>
       <c r="D6" s="9" t="s">
         <v>1</v>
       </c>
@@ -1725,11 +1725,11 @@
       <c r="BN6" s="28"/>
     </row>
     <row r="7" spans="1:66" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="59"/>
+      <c r="A7" s="44"/>
       <c r="B7" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="C7" s="58"/>
+      <c r="C7" s="43"/>
       <c r="D7" s="10" t="s">
         <v>2</v>
       </c>
@@ -6395,11 +6395,11 @@
       <c r="BN50" s="29"/>
     </row>
     <row r="51" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A51" s="60" t="s">
+      <c r="A51" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B51" s="60"/>
-      <c r="C51" s="61"/>
+      <c r="B51" s="45"/>
+      <c r="C51" s="46"/>
       <c r="D51" s="13"/>
       <c r="E51" s="12">
         <f t="shared" ref="E51:AS51" si="0">COUNTIF(E8:E50,"A")</f>
@@ -6651,11 +6651,11 @@
       </c>
     </row>
     <row r="52" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A52" s="54" t="s">
+      <c r="A52" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="B52" s="54"/>
-      <c r="C52" s="55"/>
+      <c r="B52" s="35"/>
+      <c r="C52" s="36"/>
       <c r="D52" s="13"/>
       <c r="E52" s="12">
         <f>(43-E51)</f>
@@ -6909,13 +6909,6 @@
   </sheetData>
   <autoFilter ref="N1:N52"/>
   <mergeCells count="22">
-    <mergeCell ref="A52:C52"/>
-    <mergeCell ref="Y4:AT4"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="A51:C51"/>
-    <mergeCell ref="A5:A7"/>
     <mergeCell ref="Y1:AE1"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
@@ -6931,6 +6924,13 @@
     <mergeCell ref="O1:X1"/>
     <mergeCell ref="E4:P4"/>
     <mergeCell ref="Q4:X4"/>
+    <mergeCell ref="A52:C52"/>
+    <mergeCell ref="Y4:AT4"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="A51:C51"/>
+    <mergeCell ref="A5:A7"/>
   </mergeCells>
   <conditionalFormatting sqref="E8:S50 U8:BN50">
     <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
@@ -6957,8 +6957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6973,68 +6973,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="45" t="s">
+      <c r="B1" s="67"/>
+      <c r="C1" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="45"/>
-      <c r="E1" s="46" t="s">
+      <c r="D1" s="56"/>
+      <c r="E1" s="57" t="s">
         <v>117</v>
       </c>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
     </row>
     <row r="2" spans="1:7" ht="19.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="69"/>
-      <c r="C2" s="45" t="s">
+      <c r="B2" s="63"/>
+      <c r="C2" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="45"/>
-      <c r="E2" s="46" t="s">
+      <c r="D2" s="56"/>
+      <c r="E2" s="57" t="s">
         <v>116</v>
       </c>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
     </row>
     <row r="3" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A3" s="70" t="s">
+      <c r="A3" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="70"/>
-      <c r="C3" s="45" t="s">
+      <c r="B3" s="64"/>
+      <c r="C3" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="45"/>
-      <c r="E3" s="46" t="s">
+      <c r="D3" s="56"/>
+      <c r="E3" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="68" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="56" t="s">
+      <c r="B4" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="68" t="s">
+      <c r="C4" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="68"/>
-      <c r="E4" s="68"/>
-      <c r="F4" s="68"/>
-      <c r="G4" s="68"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="62"/>
+      <c r="F4" s="62"/>
+      <c r="G4" s="62"/>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="66"/>
-      <c r="B5" s="57"/>
+      <c r="A5" s="69"/>
+      <c r="B5" s="42"/>
       <c r="C5" s="18" t="s">
         <v>14</v>
       </c>
@@ -7048,8 +7048,8 @@
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="67"/>
-      <c r="B6" s="58"/>
+      <c r="A6" s="70"/>
+      <c r="B6" s="43"/>
       <c r="C6" s="18">
         <v>25</v>
       </c>
@@ -7691,11 +7691,11 @@
         <v>22</v>
       </c>
       <c r="D38" s="26">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E38" s="26">
         <f t="shared" si="0"/>
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="F38" s="26"/>
       <c r="G38" s="26"/>
@@ -7921,10 +7921,10 @@
       <c r="G49" s="26"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="62" t="s">
+      <c r="A50" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="B50" s="63"/>
+      <c r="B50" s="66"/>
       <c r="C50" s="14"/>
       <c r="D50" s="14"/>
       <c r="E50" s="17"/>
@@ -7932,10 +7932,10 @@
       <c r="G50" s="13"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="62" t="s">
+      <c r="A51" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="B51" s="63"/>
+      <c r="B51" s="66"/>
       <c r="C51" s="14"/>
       <c r="D51" s="14"/>
       <c r="E51" s="17"/>
@@ -7943,10 +7943,10 @@
       <c r="G51" s="13"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="62" t="s">
+      <c r="A52" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="B52" s="63"/>
+      <c r="B52" s="66"/>
       <c r="C52" s="15"/>
       <c r="D52" s="14"/>
       <c r="E52" s="17"/>
@@ -7955,6 +7955,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
     <mergeCell ref="C4:G4"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
@@ -7964,12 +7970,6 @@
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="E3:G3"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:B6"/>
   </mergeCells>
   <conditionalFormatting sqref="C7:C49">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">

</xml_diff>